<commit_message>
Updated the design description as well as the BOM and the photos
</commit_message>
<xml_diff>
--- a/BOM/Bill of materials.xlsx
+++ b/BOM/Bill of materials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aregjan/git/Geiger_lanph/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F212713-FC8C-8145-A2A6-56F6B0B635B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF856646-32EE-EA40-B079-3D1DA0F55570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18600" yWindow="4720" windowWidth="41320" windowHeight="27780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="84">
   <si>
     <t>component description</t>
   </si>
@@ -127,12 +127,6 @@
     <t>https://www.digikey.com/en/products/detail/yageo/CFR-12JB-52-1M1/3927</t>
   </si>
   <si>
-    <t>5.1 kOhm</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/yageo/CFR-25JB-52-5K1/2236</t>
-  </si>
-  <si>
     <t>5.1 MOhm</t>
   </si>
   <si>
@@ -148,9 +142,6 @@
     <t>Geiger-Muller SBM-20 tube</t>
   </si>
   <si>
-    <t>https://www.ebay.com/itm/281873849954?hash=item41a0fd9e62:g:cCwAAMXQOT5Q9SYl</t>
-  </si>
-  <si>
     <t>2N3904</t>
   </si>
   <si>
@@ -278,6 +269,21 @@
   </si>
   <si>
     <t>pins, with a crimper</t>
+  </si>
+  <si>
+    <t>HV module</t>
+  </si>
+  <si>
+    <t>DAQ module</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>http://www.sovtube.com/x-ray-and-geiger-tubes/342-sbm-20u.html</t>
+  </si>
+  <si>
+    <t>or look for these on ebay</t>
   </si>
 </sst>
 </file>
@@ -375,12 +381,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -404,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -441,9 +453,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -466,6 +475,24 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -686,10 +713,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K1008"/>
+  <dimension ref="A1:K1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -698,121 +725,110 @@
     <col min="4" max="4" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:11" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="28" t="s">
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="29"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D2" s="1"/>
+      <c r="K1" s="28"/>
+    </row>
+    <row r="2" spans="1:11" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D2" s="25"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3">
-        <v>12</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="3">
-        <v>10</v>
-      </c>
-      <c r="J3" s="2">
-        <f t="shared" ref="J3:J23" si="0">C3*B3/E3</f>
-        <v>1.2</v>
-      </c>
-      <c r="K3" s="5"/>
+    <row r="3" spans="1:11" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="J3" s="36"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
+      <c r="A4" s="31" t="s">
+        <v>70</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="3">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="3">
+        <v>10</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" ref="J4:J21" si="0">C4*B4/E4</f>
+        <v>1.2</v>
+      </c>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
         <v>29.98</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E5" s="3">
         <v>100</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J5" s="2">
         <f t="shared" si="0"/>
         <v>0.29980000000000001</v>
       </c>
-      <c r="K4" s="5"/>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="3" t="s">
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B6" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C6" s="3">
         <v>10.14</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E6" s="3">
         <v>100</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J6" s="2">
         <f t="shared" si="0"/>
         <v>0.20280000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3">
-        <v>17.059999999999999</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="3">
-        <v>100</v>
-      </c>
-      <c r="J6" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17059999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -911,44 +927,47 @@
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" s="3">
-        <v>2.6</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>24</v>
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="E11" s="3">
         <v>100</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" si="0"/>
-        <v>5.2000000000000005E-2</v>
+        <v>2.2599999999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
       </c>
       <c r="C12" s="3">
-        <v>2.2599999999999998</v>
+        <v>2.6</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E12" s="3">
         <v>100</v>
       </c>
+      <c r="F12" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="J12" s="2">
-        <f t="shared" si="0"/>
-        <v>2.2599999999999999E-2</v>
+        <f>C12*B12/E12</f>
+        <v>2.6000000000000002E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -995,127 +1014,133 @@
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="3">
-        <v>2.6</v>
+        <v>64.27</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E15" s="3">
         <v>100</v>
       </c>
       <c r="J15" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.64269999999999994</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
       </c>
       <c r="C16" s="3">
-        <v>2.6</v>
+        <v>14.9</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="E16" s="3">
-        <v>100</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>15</v>
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>83</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" si="0"/>
-        <v>2.6000000000000002E-2</v>
-      </c>
+        <v>14.9</v>
+      </c>
+      <c r="K16" s="14"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
       </c>
       <c r="C17" s="3">
-        <v>64.27</v>
+        <v>16.62</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E17" s="3">
         <v>100</v>
       </c>
+      <c r="F17" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="J17" s="2">
         <f t="shared" si="0"/>
-        <v>0.64269999999999994</v>
+        <v>0.16620000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="3" t="s">
-        <v>37</v>
+      <c r="A18" s="31" t="s">
+        <v>39</v>
       </c>
       <c r="B18" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="3">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E18" s="3">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K18" s="14"/>
-    </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="20">
         <v>1</v>
       </c>
-      <c r="C19" s="3">
-        <v>16.62</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="3">
+      <c r="C19" s="20">
+        <v>13.8</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="20">
         <v>100</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>41</v>
+      <c r="F19" s="20" t="s">
+        <v>75</v>
       </c>
       <c r="J19" s="2">
         <f t="shared" si="0"/>
-        <v>0.16620000000000001</v>
+        <v>0.13800000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
       </c>
       <c r="C20" s="3">
-        <v>6</v>
-      </c>
-      <c r="D20" s="6" t="s">
+        <v>23.58</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="3">
@@ -1124,142 +1149,122 @@
       <c r="F20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:11" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" s="20">
-        <v>1</v>
-      </c>
-      <c r="C21" s="20">
-        <v>13.8</v>
-      </c>
-      <c r="D21" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" s="20">
+      <c r="J20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.23579999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="3">
+        <v>2</v>
+      </c>
+      <c r="C21" s="3">
+        <v>31.38</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="3">
         <v>100</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>78</v>
       </c>
       <c r="J21" s="2">
         <f t="shared" si="0"/>
-        <v>0.13800000000000001</v>
+        <v>0.62759999999999994</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="B22" s="3">
-        <v>1</v>
-      </c>
-      <c r="C22" s="3">
-        <v>23.58</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="3">
-        <v>100</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J22" s="2">
-        <f t="shared" si="0"/>
-        <v>0.23579999999999998</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="3" t="s">
-        <v>48</v>
+      <c r="A23" s="33" t="s">
+        <v>78</v>
       </c>
       <c r="B23" s="3">
         <v>2</v>
       </c>
       <c r="C23" s="3">
-        <v>31.38</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>49</v>
+        <v>20</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>77</v>
       </c>
       <c r="E23" s="3">
-        <v>100</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="F23" s="3"/>
       <c r="J23" s="2">
-        <f t="shared" si="0"/>
-        <v>0.62759999999999994</v>
+        <f>C23*B23/E23</f>
+        <v>0.8</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="B24" s="3">
-        <v>3</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="B25" s="3">
         <v>2</v>
       </c>
-      <c r="C25" s="3">
-        <v>20</v>
-      </c>
-      <c r="D25" s="35" t="s">
+      <c r="C24" s="3">
+        <v>11.79</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="3">
+        <v>6</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="J24" s="2">
+        <f>C24*B24/E24</f>
+        <v>3.9299999999999997</v>
+      </c>
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="25"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="5"/>
+    </row>
+    <row r="26" spans="1:11" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="5"/>
+    </row>
+    <row r="27" spans="1:11" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="E25" s="3">
-        <v>50</v>
-      </c>
-      <c r="F25" s="3"/>
-      <c r="J25" s="2">
-        <f>C25*B25/E25</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="3">
-        <v>2</v>
-      </c>
-      <c r="C26" s="3">
-        <v>11.79</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E26" s="3">
-        <v>6</v>
-      </c>
-      <c r="F26" s="3"/>
-      <c r="J26" s="2">
-        <f>C26*B26/E26</f>
-        <v>3.9299999999999997</v>
-      </c>
-      <c r="K26" s="5"/>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="D27" s="15"/>
-      <c r="F27" s="3"/>
-      <c r="J27" s="2"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="37"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="38"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B28" s="3">
         <v>1</v>
@@ -1268,13 +1273,13 @@
         <v>81.569999999999993</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E28" s="3">
         <v>10</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J28" s="2">
         <f t="shared" ref="J28:J29" si="1">C28*B28/E28</f>
@@ -1283,7 +1288,7 @@
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B29" s="3">
         <v>1</v>
@@ -1292,7 +1297,7 @@
         <v>12.04</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E29" s="3">
         <v>100</v>
@@ -1304,182 +1309,230 @@
       <c r="K29" s="5"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D30" s="1"/>
-      <c r="J30" s="2"/>
+      <c r="A30" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="3">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3">
+        <v>14.88</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" s="3">
+        <v>5</v>
+      </c>
+      <c r="J30" s="2">
+        <f>C30*B30/E30</f>
+        <v>2.976</v>
+      </c>
+      <c r="K30" s="5"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D31" s="1"/>
-      <c r="J31" s="2"/>
+      <c r="A31" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="3">
+        <v>4</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="3">
+        <v>100</v>
+      </c>
+      <c r="J31" s="2">
+        <f>C31*B31/E31</f>
+        <v>0.10400000000000001</v>
+      </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="3" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="B32" s="3">
         <v>1</v>
       </c>
-      <c r="D32" s="24"/>
-      <c r="F32" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J32" s="2"/>
-    </row>
-    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" s="3">
-        <v>1</v>
-      </c>
-      <c r="D33" s="25"/>
-      <c r="F33" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="C32" s="3">
+        <v>17.059999999999999</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="3">
+        <v>100</v>
+      </c>
+      <c r="J32" s="2">
+        <f>C32*B32/E32</f>
+        <v>0.17059999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="25"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="25"/>
       <c r="J33" s="2"/>
-    </row>
-    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B34" s="3">
-        <v>1</v>
-      </c>
-      <c r="D34" s="25"/>
-      <c r="F34" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="K33" s="5"/>
+    </row>
+    <row r="34" spans="1:11" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="25"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="25"/>
       <c r="J34" s="2"/>
-    </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35" s="3">
-        <v>1</v>
-      </c>
-      <c r="D35" s="25"/>
-      <c r="F35" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="J35" s="2"/>
+      <c r="K34" s="5"/>
+    </row>
+    <row r="35" spans="1:11" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="J35" s="36"/>
     </row>
     <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B36" s="16">
-        <v>0</v>
-      </c>
-      <c r="C36" s="3">
-        <v>7</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E36" s="3">
-        <v>40</v>
-      </c>
-      <c r="J36" s="2">
-        <f>C36*B36/E36</f>
-        <v>0</v>
-      </c>
-      <c r="K36" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="B36" s="3">
+        <v>1</v>
+      </c>
+      <c r="D36" s="39"/>
+      <c r="F36" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D37" s="1"/>
+      <c r="A37" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="3">
+        <v>1</v>
+      </c>
+      <c r="D37" s="40"/>
+      <c r="F37" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B38" s="3">
         <v>1</v>
       </c>
-      <c r="C38" s="3">
-        <v>14.88</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E38" s="3">
-        <v>5</v>
-      </c>
-      <c r="J38" s="2">
-        <f>C38*B38/E38</f>
-        <v>2.976</v>
-      </c>
-      <c r="K38" s="5"/>
+      <c r="D38" s="40"/>
+      <c r="F38" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D39" s="1"/>
+      <c r="A39" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
+      <c r="D39" s="40"/>
+      <c r="F39" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="B40" s="3">
-        <v>1</v>
+      <c r="A40" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" s="16">
+        <v>0</v>
       </c>
       <c r="C40" s="3">
-        <v>21.8</v>
+        <v>7</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E40" s="3">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="J40" s="2">
         <f>C40*B40/E40</f>
-        <v>2.7250000000000001</v>
+        <v>0</v>
       </c>
       <c r="K40" s="5"/>
     </row>
     <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="25"/>
+      <c r="A41" s="41" t="s">
+        <v>63</v>
+      </c>
       <c r="B41" s="3">
         <v>1</v>
       </c>
       <c r="C41" s="3">
-        <v>28</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>68</v>
+        <v>21.8</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="E41" s="3">
-        <v>6</v>
-      </c>
-      <c r="J41" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="J41" s="2">
+        <f>C41*B41/E41</f>
+        <v>2.7250000000000001</v>
+      </c>
       <c r="K41" s="5"/>
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="17" t="s">
-        <v>75</v>
-      </c>
+      <c r="A42" s="40"/>
       <c r="B42" s="3">
         <v>1</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="3">
+        <v>28</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E42" s="3">
+        <v>6</v>
+      </c>
+      <c r="J42" s="2"/>
+      <c r="K42" s="5"/>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="3">
+        <v>1</v>
+      </c>
+      <c r="C43">
         <v>5</v>
       </c>
-      <c r="D42" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="E42" s="20">
+      <c r="D43" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" s="20">
         <v>20</v>
       </c>
-      <c r="J42" s="2">
-        <f>C42*B42/E42</f>
+      <c r="J43" s="2">
+        <f>C43*B43/E43</f>
         <v>0.25</v>
       </c>
-      <c r="K42" s="5"/>
-    </row>
-    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="3"/>
-      <c r="D43" s="15"/>
-      <c r="J43" s="2"/>
       <c r="K43" s="5"/>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1491,29 +1544,29 @@
       <c r="J45" s="2"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C46" s="18">
+        <f>SUM(C2:C45)</f>
+        <v>657.64999999999986</v>
+      </c>
       <c r="D46" s="1"/>
       <c r="J46" s="2"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C47" s="18">
-        <f>SUM(C2:C46)</f>
-        <v>665.34999999999991</v>
+      <c r="A47" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="22"/>
+      <c r="C47" s="23">
+        <f>SUM(J2:J45)</f>
+        <v>39.800900000000006</v>
       </c>
       <c r="D47" s="1"/>
       <c r="J47" s="2"/>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B48" s="22"/>
-      <c r="C48" s="23">
-        <f>SUM(J2:J46)</f>
-        <v>44.8489</v>
-      </c>
       <c r="D48" s="1"/>
       <c r="J48" s="2"/>
     </row>
@@ -1765,7 +1818,7 @@
       <c r="D110" s="1"/>
       <c r="J110" s="2"/>
     </row>
-    <row r="111" spans="4:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="111" spans="4:10" ht="13" x14ac:dyDescent="0.15">
       <c r="D111" s="1"/>
       <c r="J111" s="2"/>
     </row>
@@ -5353,41 +5406,38 @@
       <c r="D1007" s="1"/>
       <c r="J1007" s="2"/>
     </row>
-    <row r="1008" spans="4:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="D1008" s="1"/>
-      <c r="J1008" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="A40:A41"/>
+  <mergeCells count="5">
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A35:E35"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D32" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="D7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="D8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="D9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="D10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="D12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D31" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="D13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="D14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="D15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="D16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="D17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="D19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="D20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="D22" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="D23" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="D26" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="D28" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="D29" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="D36" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="D40" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="D41" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D12" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D21" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D24" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="D28" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="D29" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D40" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="D41" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="D42" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>